<commit_message>
Picture not shown on Prod Fix
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Requirements_Analysis/Dynamic/FP-Calculation.xlsx
+++ b/Documentation/Planning/Requirements_Analysis/Dynamic/FP-Calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acs/Eigene_Dateien_Fabian/Arbeit/Studium/DHBW/Kurse/SE/BFFL/bffl/Documentation/Planning/Requirements_Analysis/Dynamic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE68E8E-A3D5-EC4C-BF52-44A3BF2D87D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534B0119-1785-CF4A-9CFD-BF2379056B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="520" windowWidth="37380" windowHeight="19500" xr2:uid="{FB18223D-5746-984A-B14B-3F8BA6F63D9B}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="37380" windowHeight="19500" activeTab="2" xr2:uid="{FB18223D-5746-984A-B14B-3F8BA6F63D9B}"/>
   </bookViews>
   <sheets>
     <sheet name="UC-Specific" sheetId="1" r:id="rId1"/>
@@ -953,13 +953,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,41 +975,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -1013,46 +1017,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1131,10 +1131,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Chart!$N$4:$N$7</c:f>
+              <c:f>Chart!$N$4:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1142,31 +1142,37 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>180</c:v>
+                <c:pt idx="4">
+                  <c:v>34.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$O$4:$O$7</c:f>
+              <c:f>Chart!$O$4:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14.29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>38.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>31.68</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>112.122</c:v>
+                <c:pt idx="4">
+                  <c:v>48.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1210,41 +1216,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Chart!$N$9:$N$12</c:f>
+              <c:f>Chart!$N$11:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>172.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62.96</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64.790000000000006</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$O$9:$O$12</c:f>
+              <c:f>Chart!$O$11:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>107.91</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>48.51</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.61</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>49.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1254,6 +1248,77 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-54C8-8647-866C-39CE5B210914}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Avg</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$N$15:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$O$15:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8609-794D-A0A4-7FF80DEFF446}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2564,7 +2629,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>226769</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2924,11 +2989,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B8FD52-783D-6D43-B7B5-5FCA89A18822}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="18" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2948,17 +3013,17 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
       <c r="M1" s="7"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
@@ -2968,36 +3033,36 @@
       <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="74"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="90"/>
     </row>
     <row r="3" spans="1:19" ht="31" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="80" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="82"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="98"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -3037,13 +3102,13 @@
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="65">
+      <c r="B5" s="76">
         <v>1</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="82" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="28" t="s">
@@ -3058,116 +3123,116 @@
       <c r="H5" s="45">
         <v>32</v>
       </c>
-      <c r="I5" s="91"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="93"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="49">
         <v>31.68</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="66"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="68" t="s">
+      <c r="B6" s="77"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="70"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="72"/>
       <c r="I6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="94"/>
+      <c r="J6" s="66"/>
       <c r="K6" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="66"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="68" t="s">
+      <c r="B7" s="77"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="70"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="72"/>
       <c r="I7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="95"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="66"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="68" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="70"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
       <c r="I8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="96"/>
+      <c r="J8" s="69"/>
       <c r="K8" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="52"/>
     </row>
     <row r="9" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="66"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="68" t="s">
+      <c r="B9" s="77"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="72"/>
       <c r="I9" s="40" t="s">
         <v>37</v>
       </c>
       <c r="J9" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="94"/>
+      <c r="K9" s="66"/>
       <c r="L9" s="52"/>
     </row>
     <row r="10" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="67"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="68" t="s">
+      <c r="B10" s="78"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="84"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="86"/>
       <c r="I10" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J10" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="97"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="53"/>
     </row>
     <row r="11" spans="1:19" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="65">
+      <c r="B11" s="76">
         <v>2</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="82" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="28" t="s">
@@ -3182,116 +3247,116 @@
       <c r="H11" s="46">
         <v>106.8309</v>
       </c>
-      <c r="I11" s="91"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="93"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="75"/>
       <c r="L11" s="49">
         <v>107.91</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="66"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="68" t="s">
+      <c r="B12" s="77"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
       <c r="I12" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="94"/>
+      <c r="J12" s="66"/>
       <c r="K12" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="66"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="68" t="s">
+      <c r="B13" s="77"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="70"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
       <c r="I13" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="95"/>
+      <c r="J13" s="68"/>
       <c r="K13" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="66"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="68" t="s">
+      <c r="B14" s="77"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="72"/>
       <c r="I14" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="96"/>
+      <c r="J14" s="69"/>
       <c r="K14" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="66"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="68" t="s">
+      <c r="B15" s="77"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="72"/>
       <c r="I15" s="40" t="s">
         <v>41</v>
       </c>
       <c r="J15" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="94"/>
+      <c r="K15" s="66"/>
       <c r="L15" s="50"/>
     </row>
     <row r="16" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="67"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="68" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="69"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="84"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="86"/>
       <c r="I16" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="97"/>
+      <c r="K16" s="67"/>
       <c r="L16" s="51"/>
     </row>
     <row r="17" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="65">
+      <c r="B17" s="76">
         <v>3</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="82" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="28" t="s">
@@ -3304,118 +3369,118 @@
         <v>20</v>
       </c>
       <c r="H17" s="46">
-        <v>48.024900000000002</v>
-      </c>
-      <c r="I17" s="91"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="93"/>
+        <v>34.75</v>
+      </c>
+      <c r="I17" s="73"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="75"/>
       <c r="L17" s="49">
         <v>48.51</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="66"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="68" t="s">
+      <c r="B18" s="77"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="70"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="72"/>
       <c r="I18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="94"/>
+      <c r="J18" s="66"/>
       <c r="K18" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L18" s="50"/>
     </row>
     <row r="19" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="66"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="68" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="70"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="72"/>
       <c r="I19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="95"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L19" s="50"/>
     </row>
     <row r="20" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="66"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="68" t="s">
+      <c r="B20" s="77"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="70"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="72"/>
       <c r="I20" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="96"/>
+      <c r="J20" s="69"/>
       <c r="K20" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L20" s="50"/>
     </row>
     <row r="21" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="66"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="68" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="70"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="72"/>
       <c r="I21" s="40" t="s">
         <v>41</v>
       </c>
       <c r="J21" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="94"/>
+      <c r="K21" s="66"/>
       <c r="L21" s="50"/>
     </row>
     <row r="22" spans="2:12" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="67"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="68" t="s">
+      <c r="B22" s="78"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="69"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="84"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="86"/>
       <c r="I22" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="97"/>
+      <c r="K22" s="67"/>
       <c r="L22" s="51"/>
     </row>
     <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="65">
+      <c r="B23" s="76">
         <v>4</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="85" t="s">
+      <c r="D23" s="82" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="28" t="s">
@@ -3428,118 +3493,118 @@
         <v>20</v>
       </c>
       <c r="H23" s="46">
-        <v>38.2239</v>
-      </c>
-      <c r="I23" s="91"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="93"/>
+        <v>18.5</v>
+      </c>
+      <c r="I23" s="73"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
       <c r="L23" s="49">
         <v>38.61</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="66"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="68" t="s">
+      <c r="B24" s="77"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="70"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="72"/>
       <c r="I24" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="94"/>
+      <c r="J24" s="66"/>
       <c r="K24" s="40" t="s">
         <v>42</v>
       </c>
       <c r="L24" s="50"/>
     </row>
     <row r="25" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="66"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="68" t="s">
+      <c r="B25" s="77"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
       <c r="I25" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="95"/>
+      <c r="J25" s="68"/>
       <c r="K25" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L25" s="50"/>
     </row>
     <row r="26" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="66"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="68" t="s">
+      <c r="B26" s="77"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="70"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="72"/>
       <c r="I26" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="96"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="50"/>
     </row>
     <row r="27" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="66"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="68" t="s">
+      <c r="B27" s="77"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="72"/>
       <c r="I27" s="40" t="s">
         <v>45</v>
       </c>
       <c r="J27" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="94"/>
+      <c r="K27" s="66"/>
       <c r="L27" s="50"/>
     </row>
     <row r="28" spans="2:12" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="67"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="68" t="s">
+      <c r="B28" s="78"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="72"/>
       <c r="I28" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J28" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="97"/>
+      <c r="K28" s="67"/>
       <c r="L28" s="54"/>
     </row>
     <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="65">
+      <c r="B29" s="76">
         <v>5</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="82" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="28" t="s">
@@ -3554,116 +3619,116 @@
       <c r="H29" s="46">
         <v>49.005000000000003</v>
       </c>
-      <c r="I29" s="91"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="93"/>
+      <c r="I29" s="73"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="75"/>
       <c r="L29" s="49">
         <v>49.5</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="66"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="68" t="s">
+      <c r="B30" s="77"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="70"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="J30" s="94"/>
+      <c r="J30" s="66"/>
       <c r="K30" s="40" t="s">
         <v>47</v>
       </c>
       <c r="L30" s="50"/>
     </row>
     <row r="31" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="66"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="68" t="s">
+      <c r="B31" s="77"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="70"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="72"/>
       <c r="I31" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="95"/>
+      <c r="J31" s="68"/>
       <c r="K31" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L31" s="50"/>
     </row>
     <row r="32" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="66"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="68" t="s">
+      <c r="B32" s="77"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="70"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="72"/>
       <c r="I32" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="96"/>
+      <c r="J32" s="69"/>
       <c r="K32" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L32" s="50"/>
     </row>
     <row r="33" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="66"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="68" t="s">
+      <c r="B33" s="77"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="70"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="72"/>
       <c r="I33" s="40" t="s">
         <v>48</v>
       </c>
       <c r="J33" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="94"/>
+      <c r="K33" s="66"/>
       <c r="L33" s="50"/>
     </row>
     <row r="34" spans="1:20" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="67"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="68" t="s">
+      <c r="B34" s="78"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="69"/>
-      <c r="G34" s="83"/>
-      <c r="H34" s="84"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="86"/>
       <c r="I34" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J34" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="97"/>
+      <c r="K34" s="67"/>
       <c r="L34" s="51"/>
     </row>
     <row r="35" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="65">
+      <c r="B35" s="76">
         <v>6</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="85" t="s">
+      <c r="D35" s="82" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="28" t="s">
@@ -3678,106 +3743,106 @@
       <c r="H35" s="46">
         <v>6.5</v>
       </c>
-      <c r="I35" s="91"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="93"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="75"/>
       <c r="L35" s="49">
         <v>17.82</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="66"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="68" t="s">
+      <c r="B36" s="77"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="70"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="72"/>
       <c r="I36" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="94"/>
+      <c r="J36" s="66"/>
       <c r="K36" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L36" s="50"/>
     </row>
     <row r="37" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="66"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="68" t="s">
+      <c r="B37" s="77"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="70"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="72"/>
       <c r="I37" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="95"/>
+      <c r="J37" s="68"/>
       <c r="K37" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L37" s="50"/>
     </row>
     <row r="38" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="66"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="68" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="72"/>
       <c r="I38" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J38" s="96"/>
+      <c r="J38" s="69"/>
       <c r="K38" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="50"/>
     </row>
     <row r="39" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="66"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="68" t="s">
+      <c r="B39" s="77"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="70"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="72"/>
       <c r="I39" s="40" t="s">
         <v>39</v>
       </c>
       <c r="J39" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="94"/>
+      <c r="K39" s="66"/>
       <c r="L39" s="50"/>
     </row>
     <row r="40" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="67"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="68" t="s">
+      <c r="B40" s="78"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="69"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="70"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="72"/>
       <c r="I40" s="40" t="s">
         <v>32</v>
       </c>
       <c r="J40" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="K40" s="96"/>
+      <c r="K40" s="69"/>
       <c r="L40" s="54"/>
     </row>
     <row r="41" spans="1:20" s="15" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4457,34 +4522,33 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="J36:J38"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="B23:B28"/>
@@ -4501,33 +4565,34 @@
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="J12:J14"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="K27:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4552,10 +4617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2945D-51D3-0249-91B2-5CC246383793}">
-  <dimension ref="M3:O32"/>
+  <dimension ref="M3:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4573,11 +4638,11 @@
         <v>0</v>
       </c>
       <c r="O4" s="57">
-        <v>14.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M5" s="98"/>
+      <c r="M5" s="65"/>
       <c r="N5" s="55">
         <f>'UC-Specific'!H35</f>
         <v>6.5</v>
@@ -4588,82 +4653,85 @@
       </c>
     </row>
     <row r="6" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N6" s="55">
+      <c r="M6" s="65"/>
+      <c r="N6" s="58">
+        <v>18.5</v>
+      </c>
+      <c r="O6" s="59">
+        <v>38.61</v>
+      </c>
+    </row>
+    <row r="7" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N7" s="55">
         <f>'UC-Specific'!H5</f>
         <v>32</v>
       </c>
-      <c r="O6" s="57">
+      <c r="O7" s="57">
         <f>'UC-Specific'!L5</f>
         <v>31.68</v>
       </c>
     </row>
-    <row r="7" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N7" s="55">
-        <v>180</v>
-      </c>
-      <c r="O7" s="57">
-        <v>112.122</v>
-      </c>
-    </row>
     <row r="8" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="58">
+        <v>34.75</v>
+      </c>
+      <c r="O8" s="59">
+        <v>48.51</v>
+      </c>
+    </row>
+    <row r="9" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N9" s="55"/>
+      <c r="O9" s="57"/>
+    </row>
+    <row r="10" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N10" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="61" t="s">
+      <c r="O10" s="61" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N9" s="58">
-        <v>172.25</v>
-      </c>
-      <c r="O9" s="59">
+    <row r="11" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N11" s="58">
+        <v>81</v>
+      </c>
+      <c r="O11" s="59">
         <f>'UC-Specific'!L11</f>
         <v>107.91</v>
       </c>
     </row>
-    <row r="10" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N10" s="58">
-        <v>62.96</v>
-      </c>
-      <c r="O10" s="59">
-        <f>'UC-Specific'!L17</f>
-        <v>48.51</v>
-      </c>
-    </row>
-    <row r="11" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N11" s="58">
-        <v>44.75</v>
-      </c>
-      <c r="O11" s="59">
-        <f>'UC-Specific'!L23</f>
-        <v>38.61</v>
-      </c>
-    </row>
     <row r="12" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N12" s="58">
-        <v>64.790000000000006</v>
-      </c>
-      <c r="O12" s="59">
+      <c r="N12" s="58"/>
+      <c r="O12" s="59"/>
+    </row>
+    <row r="13" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N13" s="58">
+        <v>37.5</v>
+      </c>
+      <c r="O13" s="59">
         <f>'UC-Specific'!L29</f>
         <v>49.5</v>
       </c>
     </row>
-    <row r="13" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N13" s="55"/>
-      <c r="O13" s="57"/>
-    </row>
     <row r="14" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="57"/>
     </row>
     <row r="15" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
+      <c r="N15" s="56">
+        <v>0</v>
+      </c>
+      <c r="O15" s="56">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
+      <c r="N16" s="56">
+        <v>90</v>
+      </c>
+      <c r="O16" s="56">
+        <v>120</v>
+      </c>
     </row>
     <row r="17" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N17" s="56"/>
@@ -4703,7 +4771,7 @@
     </row>
     <row r="26" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N26" s="56"/>
-      <c r="O26" s="64"/>
+      <c r="O26" s="56"/>
     </row>
     <row r="27" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N27" s="56"/>
@@ -4728,6 +4796,10 @@
     <row r="32" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N32" s="56"/>
       <c r="O32" s="64"/>
+    </row>
+    <row r="33" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N33" s="56"/>
+      <c r="O33" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add last UC-Documentation and Updates FP Calc
</commit_message>
<xml_diff>
--- a/Documentation/Planning/Requirements_Analysis/Dynamic/FP-Calculation.xlsx
+++ b/Documentation/Planning/Requirements_Analysis/Dynamic/FP-Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acs/Eigene_Dateien_Fabian/Arbeit/Studium/DHBW/Kurse/SE/BFFL/bffl/Documentation/Planning/Requirements_Analysis/Dynamic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534B0119-1785-CF4A-9CFD-BF2379056B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511BE94B-2F68-F140-80D6-7D8F56CA7EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="37380" windowHeight="19500" activeTab="2" xr2:uid="{FB18223D-5746-984A-B14B-3F8BA6F63D9B}"/>
+    <workbookView xWindow="-37900" yWindow="500" windowWidth="37380" windowHeight="21100" activeTab="2" xr2:uid="{FB18223D-5746-984A-B14B-3F8BA6F63D9B}"/>
   </bookViews>
   <sheets>
     <sheet name="UC-Specific" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
   <si>
     <t>Nr.</t>
   </si>
@@ -771,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -935,11 +935,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -954,17 +950,77 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -974,42 +1030,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -1131,12 +1151,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Chart!$N$4:$N$9</c:f>
+              <c:f>Chart!$N$4:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.74650000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.5</c:v>
@@ -1150,15 +1170,18 @@
                 <c:pt idx="4">
                   <c:v>34.75</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$O$4:$O$9</c:f>
+              <c:f>Chart!$O$4:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1174,6 +1197,9 @@
                 <c:pt idx="4">
                   <c:v>48.51</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>107.91</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1185,75 +1211,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Unfinished UCs</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                    <a:alpha val="70000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Chart!$N$11:$N$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Chart!$O$11:$O$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>107.91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>49.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-54C8-8647-866C-39CE5B210914}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
           <c:tx>
             <c:v>Avg</c:v>
           </c:tx>
@@ -1287,24 +1246,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Chart!$N$15:$N$16</c:f>
+              <c:f>Chart!$N$16:$N$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.74650000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>68.110299999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$O$15:$O$16</c:f>
+              <c:f>Chart!$O$16:$O$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1319,6 +1278,67 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8609-794D-A0A4-7FF80DEFF446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Unfinished UCs (Update)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>28.534099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>49.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A08D-5941-BC93-8454D6D75ADF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1337,7 +1357,7 @@
         <c:axId val="2037849375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="180"/>
+          <c:max val="120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1613,7 +1633,7 @@
         <c:crossAx val="2037849375"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="10"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1626,13 +1646,33 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.54012724756593844"/>
+          <c:y val="4.9800902757620502E-2"/>
+          <c:w val="0.19893227462310303"/>
+          <c:h val="9.7261827492803585E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2628,9 +2668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>226769</xdr:colOff>
+      <xdr:colOff>359833</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2990,10 +3030,10 @@
   <dimension ref="A1:T82"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="18" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="4" topLeftCell="S20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24:H24"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3013,17 +3053,17 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
       <c r="M1" s="7"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
@@ -3033,36 +3073,36 @@
       <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
     </row>
     <row r="3" spans="1:19" ht="31" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="91"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96" t="s">
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="98"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="102"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -3102,13 +3142,13 @@
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="76">
+      <c r="B5" s="77">
         <v>1</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="83" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="28" t="s">
@@ -3123,116 +3163,116 @@
       <c r="H5" s="45">
         <v>32</v>
       </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
       <c r="L5" s="49">
         <v>31.68</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="77"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="70" t="s">
+      <c r="B6" s="78"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="72"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="88"/>
       <c r="I6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="66"/>
+      <c r="J6" s="70"/>
       <c r="K6" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="77"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="70" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="72"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
       <c r="I7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="68"/>
+      <c r="J7" s="71"/>
       <c r="K7" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="77"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="70" t="s">
+      <c r="B8" s="78"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="88"/>
       <c r="I8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="69"/>
+      <c r="J8" s="72"/>
       <c r="K8" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="52"/>
     </row>
     <row r="9" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="77"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="70" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="72"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="88"/>
       <c r="I9" s="40" t="s">
         <v>37</v>
       </c>
       <c r="J9" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="66"/>
+      <c r="K9" s="70"/>
       <c r="L9" s="52"/>
     </row>
     <row r="10" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="78"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="70" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="86"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="90"/>
       <c r="I10" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J10" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="67"/>
+      <c r="K10" s="73"/>
       <c r="L10" s="53"/>
     </row>
     <row r="11" spans="1:19" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="76">
+      <c r="B11" s="77">
         <v>2</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="83" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="28" t="s">
@@ -3245,118 +3285,118 @@
         <v>20</v>
       </c>
       <c r="H11" s="46">
-        <v>106.8309</v>
-      </c>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="75"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
       <c r="L11" s="49">
         <v>107.91</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="77"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="70" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="72"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="88"/>
       <c r="I12" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="66"/>
+      <c r="J12" s="70"/>
       <c r="K12" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="77"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="70" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="72"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
       <c r="I13" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="68"/>
+      <c r="J13" s="71"/>
       <c r="K13" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="77"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="70" t="s">
+      <c r="B14" s="78"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="72"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
       <c r="I14" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="69"/>
+      <c r="J14" s="72"/>
       <c r="K14" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="77"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="70" t="s">
+      <c r="B15" s="78"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="72"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
       <c r="I15" s="40" t="s">
         <v>41</v>
       </c>
       <c r="J15" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="66"/>
+      <c r="K15" s="70"/>
       <c r="L15" s="50"/>
     </row>
     <row r="16" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="78"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="70" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="90"/>
       <c r="I16" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="67"/>
+      <c r="K16" s="73"/>
       <c r="L16" s="51"/>
     </row>
     <row r="17" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="76">
+      <c r="B17" s="77">
         <v>3</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="83" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="28" t="s">
@@ -3371,116 +3411,116 @@
       <c r="H17" s="46">
         <v>34.75</v>
       </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="75"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="76"/>
       <c r="L17" s="49">
         <v>48.51</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="77"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="70" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="72"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="88"/>
       <c r="I18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="66"/>
+      <c r="J18" s="70"/>
       <c r="K18" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L18" s="50"/>
     </row>
     <row r="19" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="77"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="70" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="72"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="88"/>
       <c r="I19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="68"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L19" s="50"/>
     </row>
     <row r="20" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="77"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="70" t="s">
+      <c r="B20" s="78"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="72"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="88"/>
       <c r="I20" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="69"/>
+      <c r="J20" s="72"/>
       <c r="K20" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L20" s="50"/>
     </row>
     <row r="21" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="77"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="70" t="s">
+      <c r="B21" s="78"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="72"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="88"/>
       <c r="I21" s="40" t="s">
         <v>41</v>
       </c>
       <c r="J21" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="66"/>
+      <c r="K21" s="70"/>
       <c r="L21" s="50"/>
     </row>
     <row r="22" spans="2:12" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="78"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="70" t="s">
+      <c r="B22" s="79"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="86"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="90"/>
       <c r="I22" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="67"/>
+      <c r="K22" s="73"/>
       <c r="L22" s="51"/>
     </row>
     <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="76">
+      <c r="B23" s="77">
         <v>4</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="83" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="28" t="s">
@@ -3493,118 +3533,118 @@
         <v>20</v>
       </c>
       <c r="H23" s="46">
-        <v>18.5</v>
-      </c>
-      <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="75"/>
+        <v>23</v>
+      </c>
+      <c r="I23" s="74"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="76"/>
       <c r="L23" s="49">
         <v>38.61</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="77"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="70" t="s">
+      <c r="B24" s="78"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="72"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="88"/>
       <c r="I24" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="66"/>
+      <c r="J24" s="70"/>
       <c r="K24" s="40" t="s">
         <v>42</v>
       </c>
       <c r="L24" s="50"/>
     </row>
     <row r="25" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="77"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="70" t="s">
+      <c r="B25" s="78"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="72"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="88"/>
       <c r="I25" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="68"/>
+      <c r="J25" s="71"/>
       <c r="K25" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L25" s="50"/>
     </row>
     <row r="26" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="77"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="70" t="s">
+      <c r="B26" s="78"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="72"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="88"/>
       <c r="I26" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="69"/>
+      <c r="J26" s="72"/>
       <c r="K26" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="50"/>
     </row>
     <row r="27" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="77"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="70" t="s">
+      <c r="B27" s="78"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="72"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="88"/>
       <c r="I27" s="40" t="s">
         <v>45</v>
       </c>
       <c r="J27" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="66"/>
+      <c r="K27" s="70"/>
       <c r="L27" s="50"/>
     </row>
     <row r="28" spans="2:12" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="78"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="70" t="s">
+      <c r="B28" s="79"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="72"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="88"/>
       <c r="I28" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J28" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="67"/>
+      <c r="K28" s="73"/>
       <c r="L28" s="54"/>
     </row>
     <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="76">
+      <c r="B29" s="77">
         <v>5</v>
       </c>
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="82" t="s">
+      <c r="D29" s="83" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="28" t="s">
@@ -3617,118 +3657,118 @@
         <v>20</v>
       </c>
       <c r="H29" s="46">
-        <v>49.005000000000003</v>
-      </c>
-      <c r="I29" s="73"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
+        <v>40</v>
+      </c>
+      <c r="I29" s="74"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="76"/>
       <c r="L29" s="49">
         <v>49.5</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="77"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="70" t="s">
+      <c r="B30" s="78"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="72"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="88"/>
       <c r="I30" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="J30" s="66"/>
+      <c r="J30" s="70"/>
       <c r="K30" s="40" t="s">
         <v>47</v>
       </c>
       <c r="L30" s="50"/>
     </row>
     <row r="31" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="77"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="70" t="s">
+      <c r="B31" s="78"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="72"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="88"/>
       <c r="I31" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="68"/>
+      <c r="J31" s="71"/>
       <c r="K31" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L31" s="50"/>
     </row>
     <row r="32" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="77"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="70" t="s">
+      <c r="B32" s="78"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="72"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="88"/>
       <c r="I32" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="69"/>
+      <c r="J32" s="72"/>
       <c r="K32" s="40" t="s">
         <v>39</v>
       </c>
       <c r="L32" s="50"/>
     </row>
     <row r="33" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="77"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="70" t="s">
+      <c r="B33" s="78"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="72"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="88"/>
       <c r="I33" s="40" t="s">
         <v>48</v>
       </c>
       <c r="J33" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="66"/>
+      <c r="K33" s="70"/>
       <c r="L33" s="50"/>
     </row>
     <row r="34" spans="1:20" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="78"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="70" t="s">
+      <c r="B34" s="79"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="71"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="86"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="90"/>
       <c r="I34" s="40" t="s">
         <v>35</v>
       </c>
       <c r="J34" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="67"/>
+      <c r="K34" s="73"/>
       <c r="L34" s="51"/>
     </row>
     <row r="35" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="76">
+      <c r="B35" s="77">
         <v>6</v>
       </c>
-      <c r="C35" s="79" t="s">
+      <c r="C35" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="83" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="28" t="s">
@@ -3743,106 +3783,106 @@
       <c r="H35" s="46">
         <v>6.5</v>
       </c>
-      <c r="I35" s="73"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="75"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="76"/>
       <c r="L35" s="49">
         <v>17.82</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="77"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="70" t="s">
+      <c r="B36" s="78"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="72"/>
+      <c r="F36" s="87"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="88"/>
       <c r="I36" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="66"/>
+      <c r="J36" s="70"/>
       <c r="K36" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L36" s="50"/>
     </row>
     <row r="37" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="77"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="70" t="s">
+      <c r="B37" s="78"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="72"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="88"/>
       <c r="I37" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="68"/>
+      <c r="J37" s="71"/>
       <c r="K37" s="40" t="s">
         <v>35</v>
       </c>
       <c r="L37" s="50"/>
     </row>
     <row r="38" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="77"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="70" t="s">
+      <c r="B38" s="78"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="88"/>
       <c r="I38" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J38" s="69"/>
+      <c r="J38" s="72"/>
       <c r="K38" s="40" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="50"/>
     </row>
     <row r="39" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="77"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="70" t="s">
+      <c r="B39" s="78"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="72"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="88"/>
       <c r="I39" s="40" t="s">
         <v>39</v>
       </c>
       <c r="J39" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="66"/>
+      <c r="K39" s="70"/>
       <c r="L39" s="50"/>
     </row>
     <row r="40" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="78"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="70" t="s">
+      <c r="B40" s="79"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="71"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="72"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="88"/>
       <c r="I40" s="40" t="s">
         <v>32</v>
       </c>
       <c r="J40" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="K40" s="69"/>
+      <c r="K40" s="72"/>
       <c r="L40" s="54"/>
     </row>
     <row r="41" spans="1:20" s="15" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4571,6 +4611,8 @@
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E40:H40"/>
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="C29:C34"/>
     <mergeCell ref="D29:D34"/>
@@ -4579,13 +4621,6 @@
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="E33:H33"/>
     <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="K33:K34"/>
     <mergeCell ref="J36:J38"/>
     <mergeCell ref="K39:K40"/>
     <mergeCell ref="K15:K16"/>
@@ -4593,6 +4628,11 @@
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="J24:J26"/>
     <mergeCell ref="K27:K28"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="K33:K34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4617,189 +4657,195 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2945D-51D3-0249-91B2-5CC246383793}">
-  <dimension ref="M3:O33"/>
+  <dimension ref="M3:O34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N3" s="62" t="s">
+      <c r="N3" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="63" t="s">
+      <c r="O3" s="59" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N4" s="55">
+      <c r="N4" s="62">
+        <v>0.74650000000000005</v>
+      </c>
+      <c r="O4" s="63">
         <v>0</v>
       </c>
-      <c r="O4" s="57">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M5" s="65"/>
-      <c r="N5" s="55">
+      <c r="M5" s="61"/>
+      <c r="N5" s="62">
         <f>'UC-Specific'!H35</f>
         <v>6.5</v>
       </c>
-      <c r="O5" s="57">
+      <c r="O5" s="63">
         <f>'UC-Specific'!L35</f>
         <v>17.82</v>
       </c>
     </row>
     <row r="6" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M6" s="65"/>
-      <c r="N6" s="58">
+      <c r="M6" s="61"/>
+      <c r="N6" s="64">
         <v>18.5</v>
       </c>
-      <c r="O6" s="59">
+      <c r="O6" s="65">
         <v>38.61</v>
       </c>
     </row>
     <row r="7" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N7" s="55">
+      <c r="N7" s="62">
         <f>'UC-Specific'!H5</f>
         <v>32</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="63">
         <f>'UC-Specific'!L5</f>
         <v>31.68</v>
       </c>
     </row>
     <row r="8" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N8" s="58">
+      <c r="N8" s="64">
         <v>34.75</v>
       </c>
-      <c r="O8" s="59">
+      <c r="O8" s="65">
         <v>48.51</v>
       </c>
     </row>
     <row r="9" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N9" s="55"/>
-      <c r="O9" s="57"/>
+      <c r="N9" s="64">
+        <v>50</v>
+      </c>
+      <c r="O9" s="65">
+        <v>107.91</v>
+      </c>
     </row>
     <row r="10" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="62"/>
+      <c r="O10" s="63"/>
+    </row>
+    <row r="11" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N11" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="61" t="s">
+      <c r="O11" s="57" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N11" s="58">
-        <v>81</v>
-      </c>
-      <c r="O11" s="59">
-        <f>'UC-Specific'!L11</f>
-        <v>107.91</v>
-      </c>
-    </row>
     <row r="12" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N12" s="58"/>
-      <c r="O12" s="59"/>
+      <c r="N12" s="64">
+        <v>28.534099999999999</v>
+      </c>
+      <c r="O12" s="65">
+        <v>49.5</v>
+      </c>
     </row>
     <row r="13" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N13" s="58">
-        <v>37.5</v>
-      </c>
-      <c r="O13" s="59">
-        <f>'UC-Specific'!L29</f>
-        <v>49.5</v>
-      </c>
+      <c r="N13" s="64"/>
+      <c r="O13" s="65"/>
     </row>
     <row r="14" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N14" s="55"/>
-      <c r="O14" s="57"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="65"/>
     </row>
     <row r="15" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N15" s="56">
+      <c r="N15" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15" s="67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="N16" s="68">
+        <v>0.74650000000000005</v>
+      </c>
+      <c r="O16" s="69">
         <v>0</v>
       </c>
-      <c r="O15" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="N16" s="56">
-        <v>90</v>
-      </c>
-      <c r="O16" s="56">
+    </row>
+    <row r="17" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N17" s="68">
+        <v>68.110299999999995</v>
+      </c>
+      <c r="O17" s="69">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-    </row>
     <row r="18" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="69"/>
     </row>
     <row r="19" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
     </row>
     <row r="20" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
     </row>
     <row r="21" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
     </row>
     <row r="22" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
     </row>
     <row r="23" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
     </row>
     <row r="24" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
     </row>
     <row r="25" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
     </row>
     <row r="26" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
     </row>
     <row r="27" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N27" s="56"/>
-      <c r="O27" s="64"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
     </row>
     <row r="28" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N28" s="56"/>
-      <c r="O28" s="64"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="60"/>
     </row>
     <row r="29" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N29" s="56"/>
-      <c r="O29" s="64"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="60"/>
     </row>
     <row r="30" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N30" s="56"/>
-      <c r="O30" s="64"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="60"/>
     </row>
     <row r="31" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N31" s="56"/>
-      <c r="O31" s="64"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="60"/>
     </row>
     <row r="32" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N32" s="56"/>
-      <c r="O32" s="64"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="60"/>
     </row>
     <row r="33" spans="14:15" x14ac:dyDescent="0.2">
-      <c r="N33" s="56"/>
-      <c r="O33" s="64"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="60"/>
+    </row>
+    <row r="34" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N34" s="55"/>
+      <c r="O34" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>